<commit_message>
project model & work order model export remove
</commit_message>
<xml_diff>
--- a/public/assets/excel/PRECISE_ENGINEERING.xlsx
+++ b/public/assets/excel/PRECISE_ENGINEERING.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PreciseEng2025\public\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D529949-8E1D-4E94-A37D-7D8BECE44994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03CF096F-BD6F-4EC5-AF10-B4868C44BF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,28 +31,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Customer Name</t>
   </si>
   <si>
-    <t>Created Date</t>
-  </si>
-  <si>
-    <t>Customer Code</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
-    <t>Qty</t>
+    <t>Email Id</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Phone No.</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Contact Person</t>
+  </si>
+  <si>
+    <t>GST No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -61,21 +67,9 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF212529"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -101,13 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,41 +417,51 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.77734375" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="5"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>